<commit_message>
Added book and student search functionality, along with student registration and login features.
The application now supports searching for books by ISBN, title, or author, and searching for students by ID, name, major, year, or email.
Student registration checks if a student ID already exists in the Excel database—if not, it creates a new entry.
Login verifies both the student ID and last name before granting access. Once logged in, students can view their loaned books and track borrow and return dates.
</commit_message>
<xml_diff>
--- a/LibraryManager/data/books.xlsx
+++ b/LibraryManager/data/books.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="621">
   <si>
     <t>ISBN</t>
   </si>
@@ -1868,6 +1868,15 @@
   </si>
   <si>
     <t>Fantazy</t>
+  </si>
+  <si>
+    <t>7878737878278</t>
+  </si>
+  <si>
+    <t>Castle of glow</t>
+  </si>
+  <si>
+    <t>Ariana Hustlie</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2235,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F402"/>
+  <dimension ref="A1:F403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10272,6 +10281,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="403">
+      <c r="A403" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="D403" s="0" t="s">
+        <v>617</v>
+      </c>
+      <c r="E403" s="0">
+        <v>2001</v>
+      </c>
+      <c r="F403" s="0">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>